<commit_message>
Re-pushing the Curtis/Rodriguez update
This is correcting for the last push that sent the Curtis/Rodriguez update to Arriola 2017
</commit_message>
<xml_diff>
--- a/data/primary_studies/Curtis_et_al_2022/intermediate/curtis_et_al_2022_methods.xlsx
+++ b/data/primary_studies/Curtis_et_al_2022/intermediate/curtis_et_al_2022_methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henry/Documents/CCN GitHub/CCRCN-Data-Library/data/primary_studies/Curtis_et_al_2022/intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6012DF28-0CE2-9B41-87A1-111E1AB14910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1439020C-0EA4-0041-BF21-1BBD26D77B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="500" windowWidth="27980" windowHeight="16140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="glossary" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="110">
   <si>
     <t>column_name</t>
   </si>
@@ -317,24 +317,15 @@
     <t>Any submitter defined notes on how the age depth model was created.</t>
   </si>
   <si>
-    <t>curtis_et_al_2022</t>
-  </si>
-  <si>
     <t>gouge auger</t>
   </si>
   <si>
     <t>corer limits compaction</t>
   </si>
   <si>
-    <t>is this vol of already dried material?</t>
-  </si>
-  <si>
     <t>not specified</t>
   </si>
   <si>
-    <t>methods behind paywall</t>
-  </si>
-  <si>
     <t>measured</t>
   </si>
   <si>
@@ -348,6 +339,18 @@
   </si>
   <si>
     <t>single set of methods</t>
+  </si>
+  <si>
+    <t>sediment not sieved</t>
+  </si>
+  <si>
+    <t>roots and rhizomes included</t>
+  </si>
+  <si>
+    <t>Curtis_et_al_2022</t>
+  </si>
+  <si>
+    <t>EA</t>
   </si>
 </sst>
 </file>
@@ -367,11 +370,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1337,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1477,16 +1482,22 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
         <v>99</v>
-      </c>
-      <c r="G2" t="s">
-        <v>100</v>
       </c>
       <c r="H2">
         <v>50</v>
@@ -1495,36 +1506,28 @@
         <v>72</v>
       </c>
       <c r="J2">
-        <v>5.2</v>
+        <v>212.37</v>
       </c>
       <c r="L2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="R2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S2" t="b">
         <v>1</v>
       </c>
       <c r="T2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="U2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="V2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="W2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="J3" t="s">
-        <v>101</v>
-      </c>
-      <c r="M3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>